<commit_message>
update .gitignore and exception_rules.json; enhance address simplification logic in address_finder.py
</commit_message>
<xml_diff>
--- a/address_data.xlsx
+++ b/address_data.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -19,10 +19,10 @@
   <fonts count="4">
     <font>
       <name val="新細明體"/>
+      <charset val="1"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <name val="新細明體"/>
@@ -33,16 +33,16 @@
     </font>
     <font>
       <name val="新細明體"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="細明體"/>
       <charset val="136"/>
       <family val="3"/>
       <sz val="9"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="DFKai-SB"/>
-      <family val="4"/>
-      <color theme="1"/>
-      <sz val="12"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,22 +80,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -172,10 +173,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -213,234 +214,128 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
-                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
-                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
         <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
-                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill>
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
-                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
-                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -456,132 +351,206 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.35546875" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
   <cols>
-    <col width="4" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="57.42578125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="70.42578125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="67.5703125" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="4" customWidth="1" style="1" min="1" max="1"/>
+    <col width="57.42578125" customWidth="1" style="1" min="2" max="2"/>
+    <col width="70.42578125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="67.5703125" customWidth="1" style="1" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="15" customHeight="1" s="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>序</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>查詢地址</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>完整地址</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>正規化地址(桃園市/區/里(鄰))</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="16.15" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1" s="1">
       <c r="A2" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>中壢區榮民南路234號1樓、2樓及地下一樓</t>
+          <t>長安路016號</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>桃園市中壢區仁愛里018鄰榮民南路234號1樓、2樓及地下一樓</t>
+          <t>桃園市平鎮區高雙里020鄰長安路16號</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>桃園市中壢區仁愛里榮民南路234號1樓、2樓及地下一樓</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="16.15" customHeight="1">
+          <t>桃園市平鎮區高雙里長安路16號</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1" s="1">
       <c r="A3" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>中壢區康樂路62號2樓</t>
+          <t>長安路16號</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>桃園市中壢區中榮里014鄰康樂路62號2樓</t>
+          <t>桃園市平鎮區高雙里020鄰長安路16號</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>桃園市中壢區中榮里康樂路62號2樓</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="47.25" customHeight="1">
+          <t>桃園市平鎮區高雙里長安路16號</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="47.25" customHeight="1" s="1">
       <c r="A4" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="inlineStr">
-        <is>
-          <t>桃園市中壢區致遠一路276號及278號1樓及2樓</t>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>長安路１６號</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>桃園市中壢區青埔里007鄰致遠一路276號及278號1樓及2樓</t>
+          <t>桃園市平鎮區高雙里020鄰長安路16號</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>桃園市中壢區青埔里致遠一路276號及278號1樓及2樓</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="16.15" customHeight="1">
+          <t>桃園市平鎮區高雙里長安路16號</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1" s="1">
       <c r="A5" t="n">
         <v>4</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>中壢區後興路一段25號1樓及2樓</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>桃園市中壢區至善里002鄰後興路一段25號1樓及2樓</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>桃園市中壢區至善里後興路一段25號1樓及2樓</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+      <c r="B5" s="4" t="n"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+    </row>
+    <row r="6" ht="15" customHeight="1" s="1">
       <c r="A6" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="n"/>
+      <c r="B6" s="4" t="n"/>
       <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr"/>
     </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="n"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
+    </row>
+    <row r="18" ht="30" customHeight="1" s="1">
+      <c r="A18" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="4" t="n"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
refactor: enhance Chrome driver setup to suppress logs and console window
</commit_message>
<xml_diff>
--- a/address_data.xlsx
+++ b/address_data.xlsx
@@ -80,7 +80,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -88,9 +88,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -351,10 +348,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.35546875" defaultRowHeight="15" customHeight="1" outlineLevelCol="0"/>
@@ -413,27 +410,27 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>長安路16號</t>
+          <t>長安路三段１６號</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>桃園市平鎮區高雙里020鄰長安路16號</t>
+          <t>查無結果</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>桃園市平鎮區高雙里長安路16號</t>
+          <t>查詢失敗</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="47.25" customHeight="1" s="1">
+    <row r="4" ht="15.75" customHeight="1" s="1">
       <c r="A4" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>長安路１６號</t>
+          <t>長安路016號</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -446,108 +443,6 @@
           <t>桃園市平鎮區高雙里長安路16號</t>
         </is>
       </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1" s="1">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="4" t="n"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-    </row>
-    <row r="6" ht="15" customHeight="1" s="1">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" s="4" t="n"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="n"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-    </row>
-    <row r="18" ht="30" customHeight="1" s="1">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" s="4" t="n"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>